<commit_message>
Fixed few excel bugs
</commit_message>
<xml_diff>
--- a/public/storage/ExcelFiles/PackageMenu/SinglePackageMenuExcelFormat.xlsx
+++ b/public/storage/ExcelFiles/PackageMenu/SinglePackageMenuExcelFormat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szaid\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Hyplap\P-2 POONAM KAPOOR\PoonamKapurv2\public\storage\ExcelFiles\PackageMenu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9772E16-E6B1-419A-A633-69655BDF9B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199468F8-A3F5-4C62-B0B3-0C468478B2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8928" xr2:uid="{FA9AEA4B-541F-4F43-86BD-CF8F858E8DA3}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{FA9AEA4B-541F-4F43-86BD-CF8F858E8DA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -427,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{188B6567-97B1-4608-8372-9B2187EEABFA}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,6 +451,161 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>